<commit_message>
update data and notebook
</commit_message>
<xml_diff>
--- a/techxchange/2024-watsonx-handson-1/data/TechXchangeJapan2024.xlsx
+++ b/techxchange/2024-watsonx-handson-1/data/TechXchangeJapan2024.xlsx
@@ -1212,7 +1212,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>お客様講師</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Automationテクニカル・スペシャリスト 平岡 大祐</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1412,17 +1412,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>10-1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>お客様講演</t>
+          <t>iPaaS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Think 2024およびTechXchange 2024 フィードバック</t>
+          <t>進化するIBM iPaaS、ニューフェースを迎えてHybrid iPaaSへ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1432,13 +1432,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2F 華しずか</t>
+          <t>4F 平安</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>今年海外で開催されたIBMのメインイベントであるThink 2024とTechXchange 2024のフィードバックセッションです。
-生成形AIを中心としたIBMの戦略と最新のテクノロジーを紹介します。またそのような最新テクノロジーに取り組む技術者の動向を含めて、イベントの雰囲気を肌で感じ取っていただけるセッションです。</t>
+          <t>本セッションでは、新たにIBMの仲間となったwebMethodsを活用し、多様なデータを手軽に連携するiPaaS(Integration Platform as a Service)の価値を紹介します。ビジネスに役立つAIのためにはオンプレミスかクラウドかを問わず、多様な環境に散在するデータを柔軟に連携する必要があります。IBMが目指すHybrid iPaaSとは何なのか、その魅力に迫ります。*当セッションは軽食を食べながら受講いただけます。</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1448,7 +1447,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 TBD TBD TBD</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Automation事業部 プリンシパル・ブランド・セールス・スペシャリスト 早川 ゆき</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1460,17 +1459,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>10-2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>お客様講演</t>
+          <t>iPaaS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>エッジAIセンシングプラットフォームとMaximo/TRIRIGAによる業務スペース活用効率化</t>
+          <t>iPaaSで今すぐ始める、手軽なITモダナイゼーション</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1480,12 +1479,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2F 華しずか</t>
+          <t>4F 平安</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>快適な職場環境は従業員の生産性や満足度向上に貢献するものであり、無駄な専有状況や過剰な混雑はそれを妨げる課題であり、不動産コストにも影響します。この課題解決に貢献するソニー製のエッジAIセンシングプラットフォームとMaximo Monitor/TRIRIGAによる共創ソリューションをご紹介するとともに、本ソリューションにおける技術的な特徴についてご説明します。</t>
+          <t>iPaaS(Integration Platform as a Service)を活用して、今すぐ始められる手軽なITモダナイゼーションを実現しませんか。webMethodsにより、コンテナ技術やAI時代に必要なITモダナイズを実現させることで、柔軟でスケーラブルなシステムを短期間で構築することが可能です。業務効率を飛躍的に向上させ、競争力を強化することも可能です。デモを通じて、迅速かつ確実なデジタル・トランスフォーメーションの方法を具体的にご説明いたします。</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1495,7 +1494,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>お客様講師, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 Sustainabilityテクニカル・スペシャリスト 今井 悠, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 アカウント・テクニカル・リーダー 今関 俊行</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Automation事業部 シニア・ソリューション・アーキテクト 小野 奈海</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1507,7 +1506,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1517,12 +1516,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>三菱UFJ銀行の勘定系モダナイゼーション事例</t>
+          <t>Think 2024およびTechXchange 2024 フィードバック</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14:00-14:40</t>
+          <t>12:00-12:40</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1532,7 +1531,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>三菱UFJ銀行の勘定系システムは長年稼働する中で、チャネル拡大や商品・サービス追加などに既存プログラムを大幅に変更することなく継ぎ接ぎ対応をした結果、複雑化・肥大化が進みました。当課題解消のため、メインフレームとオープン基盤を適材適所で利用する“ハイブリッドアーキテクチャ・モダナイゼーション”を実践中です。本セッションにて、オープン基盤上で再構築する“勘定系フロント”の概要についてご紹介します。</t>
+          <t>今年海外で開催されたIBMのメインイベントであるThink 2024とTechXchange 2024のフィードバックセッションです。生成形AIを中心としたIBMの戦略と最新のテクノロジーを紹介します。またそのような最新テクノロジーに取り組む技術者の動向を含めて、イベントの雰囲気を肌で感じ取っていただけるセッションです。</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1542,7 +1541,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>お客様講師, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 アカウント・テクニカル・リーダー 奥野 将嘉</t>
+          <t>お客様講師, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 執行役員 野波 衆太郎, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 クライアント・エンジニアリング事業部 クライアント・エンジニアリング・ソリューション・アーキテクト 野村 幸平</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1554,7 +1553,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1564,12 +1563,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>関西電力流 FinOps(クラウドコスト最適化)の実践</t>
+          <t>エッジAIセンシングプラットフォームとMaximo/TRIRIGAによる業務スペース活用効率化</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15:00-15:40</t>
+          <t>13:00-13:40</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1579,7 +1578,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>関西電力グループは、お客さまと社会に新しい価値をお届けするため、エネルギー分野にとどまらず、日々進化するテクノロジーをいち早く取り入れ、次代をつくりだす企業を目指しています。さらなるクラウドの活用や、パフォーマンス維持とリソース最適利用の両立にはクラウドリソースのデータ可視化が必要でした。CCoEとして取り組んでいるIBM Turbonomicを活用したFinOps実践活動についてお話しします。</t>
+          <t>快適な職場環境は従業員の生産性や満足度向上に貢献するものであり、無駄な専有状況や過剰な混雑はそれを妨げる課題であり、不動産コストにも影響します。この課題解決に貢献するソニー製のエッジAIセンシングプラットフォームとMaximo Monitor/TRIRIGAによる共創ソリューションをご紹介するとともに、本ソリューションにおける技術的な特徴についてご説明します。</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1589,7 +1588,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>お客様講師</t>
+          <t>お客様講師, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 サステナビリティ・ソフトウェア テクニカル・スペシャリスト 今井 悠, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 アカウント・テクニカル・リーダー 今関 俊行</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1601,7 +1600,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1611,12 +1610,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DXのためのデータ活用基盤</t>
+          <t>三菱UFJ銀行の勘定系モダナイゼーション事例</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>16:00-16:40</t>
+          <t>14:00-14:40</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1626,7 +1625,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>かんぽ生命ではDXのためのシステム基盤整備を進めています。この取り組みの中から、基幹系データへの効率的なアクセスの実現、全社的な分析環境の整備、AI活用等今後の展望についてご紹介します。</t>
+          <t>三菱UFJ銀行の勘定系システムは長年稼働する中で、チャネル拡大や商品・サービス追加などに既存プログラムを大幅に変更することなく継ぎ接ぎ対応をした結果、複雑化・肥大化が進みました。当課題解消のため、メインフレームとオープン基盤を適材適所で利用する“ハイブリッドアーキテクチャ・モダナイゼーション”を実践中です。本セッションにて、オープン基盤上で再構築する“勘定系フロント”の概要についてご紹介します。</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1636,7 +1635,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>お客様講師</t>
+          <t>お客様講師, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 アカウント・テクニカル・リーダー 奥野 将嘉</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1648,7 +1647,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2-6</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1658,12 +1657,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>生成AI×データ分析がUXの解像度を上げる</t>
+          <t>関西電力流 FinOps(クラウドコスト最適化)の実践</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>17:00-17:40</t>
+          <t>15:00-15:40</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1673,9 +1672,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>生成AIは、テキスト分析にもブレイクスルーをもたらし、従来は手間を要した分析を、すぐに・容易に行うことが出来るようになりました。
-近年生成AIの陰に隠れがちな機械学習・データ分析の技術は依然として重要であるだけでなく、生成AIによるテキスト分析と併用することで、CX,EX等、UXのより深い調査を可能にします。
-社内調査で試みたデータ分析事例を元に、生成AI×データ分析によるUX理解の試み・展望をご紹介します。</t>
+          <t>関西電力グループは、お客さまと社会に新しい価値をお届けするため、エネルギー分野にとどまらず、日々進化するテクノロジーをいち早く取り入れ、次代をつくりだす企業を目指しています。さらなるクラウドの活用や、パフォーマンス維持とリソース最適利用の両立にはクラウドリソースのデータ可視化が必要でした。CCoEとして取り組んでいるIBM Turbonomicを活用したFinOps実践活動についてお話しします。</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1697,32 +1694,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Storage</t>
+          <t>お客様講演</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>AI が実現するランサムウェア脅威の検知とデータ・マイグレーション</t>
+          <t xml:space="preserve"> DXのためのデータ活用基盤</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>12:00-12:40</t>
+          <t>16:00-16:40</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3F シリウス</t>
+          <t>2F 華しずか</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ランサムウェア攻撃を受けた場合、如何に迅速な復旧を実現できるかがビジネスの生命線となっています。ストレージに書き込まれたデータから改変不可のコピー（スナップショット）を自動的に作成したうえで、AIがランサムウェア脅威を検知するデモをします。また、複数のストレージ間で容量や I/O 負荷を AI 予測に基づき平準化を可能とする機能を用いた新たな運用を提案します。</t>
+          <t>かんぽ生命ではDXのためのシステム基盤整備を進めています。この取り組みの中から、基幹系データへの効率的なアクセスの実現、全社的な分析環境の整備、AI活用等今後の展望についてご紹介します。</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1732,7 +1729,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 ストレージ・テクニカル・スペシャリスト 松原 圭吾</t>
+          <t>お客様講師, お客様講師</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1744,32 +1741,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>2-6</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Storage</t>
+          <t>お客様講演</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>将来を見据えた次世代AI/分析向けストレージ基盤とは</t>
+          <t>生成AI×データ分析がUXの解像度を上げる</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13:00-13:40</t>
+          <t>17:00-17:40</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3F シリウス</t>
+          <t>2F 華しずか</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>「AI 利活用の推進」、「仮想マシン環境の行く末」、「莫大なデータの保管コスト増」などのお悩みを解決する次世代プラットフォームをご紹介します。単純なインフラ更改ではなく、GPU のパフォーマンスを最大化するストレージ、仮想マシンとコンテナの統合プラットフォームなど、真の次世代インフラを追い求めましょう。</t>
+          <t>生成AIは、テキスト分析にもブレイクスルーをもたらし、従来は手間を要した分析を、すぐに・容易に行うことが出来るようになりました。近年生成AIの陰に隠れがちな機械学習・データ分析の技術は依然として重要であるだけでなく、生成AIによるテキスト分析と併用することで、CX,EX等、UXのより深い調査を可能にします。社内調査で試みたデータ分析事例を元に、生成AI×データ分析によるUX理解の試み・展望をご紹介します。</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1779,7 +1776,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 ストレージ・テクニカル・スペシャリスト 田中 裕之, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 ストレージ・テクニカル・スペシャリスト 吉岡 秀</t>
+          <t>お客様講師</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1791,22 +1788,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3-3</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Power</t>
+          <t>Storage</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>オンプレミス/エッジAIで使えるIBM Powerの最新テクノロジーを体感しよう</t>
+          <t>AI が実現するランサムウェア脅威の検知とデータ・マイグレーション</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14:00-14:40</t>
+          <t>12:00-12:40</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1816,7 +1813,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>どこにあってもAIが利用できるという状況が実現されつつあり、オンプレミスやエッジでの利用を検討するケースが増えてきています。その際、プロジェクトを成功裡に進めるために、コストパフォーマンスの良い推論環境を、セキュアに迅速に展開することが重要な検討項目になります。IBM PowerとHugging FaceやRed Hat AIの組み合わせを活用して作る、フットプリントの小さいAI推論環境の構築や活用例を事例やデモを通じて紹介します。</t>
+          <t>ランサムウェア攻撃を受けた場合、如何に迅速な復旧を実現できるかがビジネスの生命線となっています。ストレージに書き込まれたデータから改変不可のコピー（スナップショット）を自動的に作成したうえで、AIがランサムウェア脅威を検知するデモをします。また、複数のストレージ間で容量や I/O 負荷を AI 予測に基づき平準化を可能とする機能を用いた新たな運用を提案します。</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1826,7 +1823,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 IBM Powerテクニカル・スペシャリスト 伊東 大地</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 ストレージ・テクニカル・スペシャリスト 松原 圭吾</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1838,22 +1835,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Power</t>
+          <t>Storage</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>“生成AI × IBM i” - IBM i 開発方法を今、さくっとアップデートしよう</t>
+          <t>将来を見据えた次世代AI/分析向けストレージ基盤とは</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>15:00-15:40</t>
+          <t>13:00-13:40</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1863,10 +1860,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>昨今IBM i Merlin、RDi、VSCode開発などIBM i 開発環境はどんどん進化しています。
-さらにAIを用いることで、開発環境だけでなく、開発方法自体も進化していることをご存知でしょうか。
-本セッションでは、新機能であるコード・アシスタントの紹介および、IBM i 環境で、RPGのコード生成等、生産性をあげる新しい開発方法をデモンストレーションを通じてご説明します。
-「簡単に、素早く、快適なIBM i の開発方法にアップデートする」第一歩のセッションです。ぜひご参加ください。</t>
+          <t>「AI 利活用の推進」、「仮想マシン環境の行く末」、「莫大なデータの保管コスト増」などのお悩みを解決する次世代プラットフォームをご紹介します。単純なインフラ更改ではなく、GPU のパフォーマンスを最大化するストレージ、仮想マシンとコンテナの統合プラットフォームなど、真の次世代インフラを追い求めましょう。</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1876,7 +1870,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 IBM Powerテクニカル・スペシャリスト 古閑 さくら, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 IBM Powerテクニカル・スペシャリスト 肥沼 沙織</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 ストレージ・テクニカル・スペシャリスト 田中 裕之, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 ストレージ・テクニカル・スペシャリスト 吉岡 秀</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1888,22 +1882,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>3-3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mainframe</t>
+          <t>Power</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>メインフレームとAI技術 - 課題解決の新たなアプローチ</t>
+          <t>オンプレミス/エッジAIで使えるIBM Powerの最新テクノロジーを体感しよう</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>16:00-16:40</t>
+          <t>14:00-14:40</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1913,7 +1907,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>IBMメインフレームは、生誕60周年を迎えた今日においても、お客様の基幹業務を支える事はもちろんさらに活用の幅を広げています。一方で長期に渡り稼働するメインフレームならではの課題も存在します。その課題は最新のAI技術を活用して解決することが可能です。当セッションでは、メインフレーム資産の活用や運用に取り入れられているAI技術や製品が登場した背景と狙いについて、わかりやすく解説します。</t>
+          <t>どこにあってもAIが利用できるという状況が実現されつつあり、オンプレミスやエッジでの利用を検討するケースが増えてきています。その際、プロジェクトを成功裡に進めるために、コストパフォーマンスの良い推論環境を、セキュアに迅速に展開することが重要な検討項目になります。IBM PowerとHugging FaceやRed Hat AIの組み合わせを活用して作る、フットプリントの小さいAI推論環境の構築や活用例を事例やデモを通じて紹介します。</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1923,7 +1917,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Mainframeテクニカル・スペシャリスト 竹吉 俊輔</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 IBM Powerテクニカル・スペシャリスト 伊東 大地</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1935,22 +1929,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3-6</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mainframe</t>
+          <t>Power</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>メインフレーム・モダナイゼーションを加速するAI活用術</t>
+          <t>“生成AI × IBM i” - IBM i 開発方法を今、さくっとアップデートしよう</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>17:00-17:40</t>
+          <t>15:00-15:40</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1960,7 +1954,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>AIを賢く活用してメインフレーム・モダナイゼーションを実現しませんか。より身近になったAI技術はこれからの我々の働き方に様々な選択肢を与え、スキル育成や生産性向上の観点で大きな影響を与えます。今まで以上にモダナイゼーションを加速させるために、今話題のメインフレーム・アプリケーション開発に生成AIを活用できる「IBM watsonx Code Assistant for Z」を中心に、デモを交えてご紹介します。</t>
+          <t>昨今IBM i Merlin、RDi、VSCode開発などIBM i 開発環境はどんどん進化しています。さらにAIを用いることで、開発環境だけでなく、開発方法自体も進化していることをご存知でしょうか。本セッションでは、新機能であるコード・アシスタントの紹介および、IBM i 環境で、RPGのコード生成等、生産性をあげる新しい開発方法をデモンストレーションを通じてご説明します。「簡単に、素早く、快適なIBM i の開発方法にアップデートする」第一歩のセッションです。ぜひご参加ください。</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1970,7 +1964,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Mainframeテクニカル・スペシャリスト 寺村 美千賀, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 Mainframeテクニカル・スペシャリスト 三上 鉉人</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 IBM Powerテクニカル・スペシャリスト 古閑 さくら, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 IBM Powerテクニカル・スペシャリスト 肥沼 沙織</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1982,32 +1976,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4-1</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cloud</t>
+          <t>Mainframe</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>watsonxと繋がるIBM Cloudのあの手この手</t>
+          <t>メインフレームとAI技術 - 課題解決の新たなアプローチ</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12:00-12:40</t>
+          <t>16:00-16:40</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3F オリオン</t>
+          <t>3F シリウス</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>プロンプトによる生成AI活用からRetrieval-Augmented Generation(RAG)を用いた知識探索、モデル改善を目指すファイン・チューニング等、watsonxを利用してみたいお客様必見です。そもそもwatsonxとアプリケーションを繋げるために、どんなIBM Cloud構成が取れるかを解説します。なるべく安価な構成にするには、セキュアな通信を保つには、安定稼働を実現するには、など様々な構成を一挙にご紹介します。</t>
+          <t>IBMメインフレームは、生誕60周年を迎えた今日においても、お客様の基幹業務を支える事はもちろんさらに活用の幅を広げています。一方で長期に渡り稼働するメインフレームならではの課題も存在します。その課題は最新のAI技術を活用して解決することが可能です。当セッションでは、メインフレーム資産の活用や運用に取り入れられているAI技術や製品が登場した背景と狙いについて、わかりやすく解説します。</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2017,8 +2011,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 
-Cloud Platformテクニカル・スペシャリスト 片岡 弘貴</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Mainframeテクニカル・スペシャリスト 竹吉 俊輔</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2030,32 +2023,32 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>3-6</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cloud</t>
+          <t>Mainframe</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>どうするVMware、IBM Cloudを用いた最適化戦略</t>
+          <t>メインフレーム・モダナイゼーションを加速するAI活用術</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13:00-13:40</t>
+          <t>17:00-17:40</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3F オリオン</t>
+          <t>3F シリウス</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>年初から業界を賑わせているBroadcom社によるVMwareライセンスポリシーの変更に伴い、現行VMware環境上で動くワークロードのあるべき姿に対して改めて検討をされている企業は多いと思われます。本セッションでは、IBM Cloudが提供する豊富な選択肢を改めて整理し、コスト・リスク・柔軟性の観点から今後のアーキテクチャーを描く上で役立つソリューションをご紹介します。</t>
+          <t>AIを賢く活用してメインフレーム・モダナイゼーションを実現しませんか。より身近になったAI技術はこれからの我々の働き方に様々な選択肢を与え、スキル育成や生産性向上の観点で大きな影響を与えます。今まで以上にモダナイゼーションを加速させるために、今話題のメインフレーム・アプリケーション開発に生成AIを活用できる「IBM watsonx Code Assistant for Z」を中心に、デモを交えてご紹介します。</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2065,9 +2058,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 
-Cloud Platformテクニカル・スペシャリスト 安田 忍, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 
-Cloud Platformテクニカル・スペシャリスト 鶴田 萌花</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Mainframeテクニカル・スペシャリスト 寺村 美千賀, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 Mainframeテクニカル・スペシャリスト 三上 鉉人</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2079,22 +2070,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>Cloud</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>量子コンピューティング時代にむけて、今から取り組むべきセキュリティー対策</t>
+          <t>watsonxと繋がるIBM Cloudのあの手この手</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14:00-14:40</t>
+          <t>12:00-12:40</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2104,18 +2095,17 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>量子技術は企業に計り知れないほど大きな利益をもたらすポテンシャルを秘めており、社会に大きな影響を及ぼすと考えられています。その反面、現在のセキュリティー対策の根幹を支えている暗号技術に影響を及ぼす可能性があると言われています。
-このセッションでは、国内外の先行事例をもとに、企業が取るべき耐量子コンピューティング戦略とセキュリティー対策の勘所に関してご説明します。</t>
+          <t>プロンプトによる生成AI活用からRetrieval-Augmented Generation(RAG)を用いた知識探索、モデル改善を目指すファイン・チューニング等、watsonxを利用してみたいお客様必見です。そもそもwatsonxとアプリケーションを繋げるために、どんなIBM Cloud構成が取れるかを解説します。なるべく安価な構成にするには、セキュアな通信を保つには、安定稼働を実現するには、など様々な構成を一挙にご紹介します。</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>中級者</t>
+          <t>全員</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 Strategy Consulting Partner 西林 泰如</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部  Cloud Platformテクニカル・スペシャリスト 片岡 弘貴</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2127,22 +2117,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t>Cloud</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>量子コンピューティング時代にむけて、今から取り組むべきセキュリティー対策</t>
+          <t>どうするVMware、IBM Cloudを用いた最適化戦略</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14:00-14:40</t>
+          <t>13:00-13:40</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2152,18 +2142,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>量子技術は企業に計り知れないほど大きな利益をもたらすポテンシャルを秘めており、社会に大きな影響を及ぼすと考えられています。その反面、現在のセキュリティー対策の根幹を支えている暗号技術に影響を及ぼす可能性があると言われています。このセッションでは、国内外の先行事例をもとに、企業が取るべき耐量子コンピューティング戦略とセキュリティー対策の勘所に関してご説明します。</t>
+          <t>年初から業界を賑わせているBroadcom社によるVMwareライセンスポリシーの変更に伴い、現行VMware環境上で動くワークロードのあるべき姿に対して改めて検討をされている企業は多いと思われます。本セッションでは、IBM Cloudが提供する豊富な選択肢を改めて整理し、コスト・リスク・柔軟性の観点から今後のアーキテクチャーを描く上で役立つソリューションをご紹介します。</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>中級者</t>
+          <t>全員</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 コンサルティング事業本部 サイバーセキュリティー・サービス
-技術理事 大西 克美</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部  Cloud Platformテクニカル・スペシャリスト 安田 忍, 日本アイ・ビー・エム株式会社 テクノロジー事業本部  Cloud Platformテクニカル・スペシャリスト 鶴田 萌花</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2175,7 +2164,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2185,12 +2174,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>生成AI時代に考えるべきデータ・セキュリティー</t>
+          <t>量子コンピューティング時代にむけて、今から取り組むべきセキュリティー対策</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15:00-15:40</t>
+          <t>14:00-14:40</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2200,17 +2189,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>大規模言語モデルの登場や自然言語処理の進歩により、ビジネスにおける生成AIの活用が進んでおります。本セッションでは、データ・セキュリティーの観点から生成AI時代におけるセキュリティー課題を分析し、管理が必要となる項目を整理させていただきます。併せて最新のTechnologyでこの領域における課題をどのように解決していくのかをご説明します。</t>
+          <t>量子技術は企業に計り知れないほど大きな利益をもたらすポテンシャルを秘めており、社会に大きな影響を及ぼすと考えられています。その反面、現在のセキュリティー対策の根幹を支えている暗号技術に影響を及ぼす可能性があると言われています。このセッションでは、国内外の先行事例をもとに、企業が取るべき耐量子コンピューティング戦略とセキュリティー対策の勘所に関してご説明します。</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>全員</t>
+          <t>中級者</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 セキュリティー・テクニカル・スペシャリスト 吉田 剛, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 セキュリティー・テクニカル・スペシャリスト 清水 颯太</t>
+          <t>日本アイ・ビー・エム株式会社 コンサルティング事業本部 サイバーセキュリティー・サービス 技術理事 大西 克美, 日本アイ・ビー・エム株式会社 Strategy Consulting Partner 西林 泰如</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2222,22 +2211,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>4-4</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sustainability Software</t>
+          <t>Security</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Maximoと生成AIが切り拓く新たな可能性</t>
+          <t>生成AI時代に考えるべきデータ・セキュリティー</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>16:00-16:40</t>
+          <t>15:00-15:40</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2247,7 +2236,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>本セッションでは、企業資産管理ソリューションの効果的な利用方法とこれまであった課題、特に現場の手間がかかり使いこなせない問題、そのギャップを埋める生成AIの活用方法を紹介します。具体的な生成AIの実例やEAM（企業資産管理）でのデータ管理・活用、APM（資産パフォーマンス管理）における生成AIのユースケースも取り上げます。ソリューションの効果的な活用と生成AIによる可能性について深く掘り下げるセッションです。</t>
+          <t>大規模言語モデルの登場や自然言語処理の進歩により、ビジネスにおける生成AIの活用が進んでおります。本セッションでは、データ・セキュリティーの観点から生成AI時代におけるセキュリティー課題を分析し、管理が必要となる項目を整理させていただきます。併せて最新のTechnologyでこの領域における課題をどのように解決していくのかをご説明します。</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2257,8 +2246,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 Maximoエキスパート・ラボ アプリケーション・コンサルタント 横山 智史, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 
-クライアント・エンジニアリング事業部 AI エンジニア 藤井 涼平, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 Sustainabilityテクニカル・スペシャリスト 今井 悠</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 セキュリティー・テクニカル・スペシャリスト 吉田 剛, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 セキュリティー・テクニカル・スペシャリスト 清水 颯太</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2290,7 +2278,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4F オリオン</t>
+          <t>3F オリオン</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2305,7 +2293,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Sustainabilityテクニカル・スペシャリスト 藤 泉也</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 Maximoエキスパート・ラボ デリバリー・コンサルタント 横山 智史, 日本アイ・ビー・エム株式会社 テクノロジー事業本部  クライアント・エンジニアリング  AI エンジニア 藤井 涼平, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 サステナビリティ・ソフトウェア テクニカル・スペシャリスト 今井 悠</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2540,7 +2528,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 watsonx事業部 Data&amp;AIテクニカル・スペシャリスト 坂本 康輔</t>
+          <t>日本アイ・ビー・エム株式会社 テクノロジー事業本部 watsonx事業部 Data&amp;AIテクニカル・スペシャリスト 坂本 康輔, 日本アイ・ビー・エム株式会社 テクノロジー事業本部 watsonx事業部 Data&amp;AIテクニカル・スペシャリスト 西澤 賢吾</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2577,8 +2565,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>生成AIによる業務効率化の模索・実践が進んでいます。汎用ツールによる個人での業務改善だけでなく、業務に特化したツールの活用がさらなる生産性向上につながります。
-本セッションでは、顧客サービス、アプリケーション最新化、ビジネス・データ分析の各領域での対話型UIを使ったAIによる業務のサポート・自動化をデモを交えてご紹介します。</t>
+          <t>生成AIによる業務効率化の模索・実践が進んでいます。汎用ツールによる個人での業務改善だけでなく、業務に特化したツールの活用がさらなる生産性向上につながります。本セッションでは、顧客サービス、アプリケーション最新化、ビジネス・データ分析の各領域での対話型UIを使ったAIによる業務のサポート・自動化をデモを交えてご紹介します。</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2892,7 +2879,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>高信頼/コスト最適なOracle Database基盤のためのLinuxONE活用</t>
+          <t>LinuxONEによるOracle Database基盤のアジリティ/コスト効率向上</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2907,8 +2894,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>日立製作所ではお客様のシステムマイグレーション・ITモダナイゼーションを加速するソリューションを展開しております。
-このセッションでは、特に課題となる基幹系データベース基盤の移行に対して、LinuxONEと日立ストレージVSPを組合わせた高信頼性とコスト最適化を両立するOracle Databaseベストプラクティス構成と、それを実現するソリューションおよび検証結果をご紹介します。</t>
+          <t>日立製作所ではお客様のシステムマイグレーション・ITモダナイゼーションを加速するソリューションを展開しております。このセッションでは、特に課題となる基幹系データベース基盤の移行に対して、LinuxONEと日立ストレージVSPを組合わせた高信頼性とコスト最適化を両立するOracle Databaseベストプラクティス構成と、それを実現するソリューションおよび検証結果をご紹介します。</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3237,9 +3223,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>生成AIの回答精度を向上させるために、自社内のデータを活用しませんか。
-このハンズオンでは、ベクトル・データーベースを使ったRAGの基本を学びます。
-データとAIのためのオープンなデータレイクハウス watsonx.dataに含まれるベクトル・データベース Milvusを使って、生成AIで新しいデータ探索を体験してみましょう。</t>
+          <t>生成AIの回答精度を向上させるために、自社内のデータを活用しませんか。このハンズオンでは、ベクトル・データーベースを使ったRAGの基本を学びます。データとAIのためのオープンなデータレイクハウス watsonx.dataに含まれるベクトル・データベース Milvusを使って、生成AIで新しいデータ探索を体験してみましょう。</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3333,9 +3317,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>多くの企業が生成AI・基盤モデルのビジネス活用を加速していく中、AIリスク管理の重要性も高まっています。
-watsonx.governanceは企業におけるAIライフサイクル管理を通して、信頼できるAIを実現するツールキットを提供します。
-本ハンズオンではwatsonx.governanceを用いたAIリスク管理の流れを体感いただけます。</t>
+          <t>多くの企業が生成AI・基盤モデルのビジネス活用を加速していく中、AIリスク管理の重要性も高まっています。watsonx.governanceは企業におけるAIライフサイクル管理を通して、信頼できるAIを実現するツールキットを提供します。本ハンズオンではwatsonx.governanceを用いたAIリスク管理の流れを体感いただけます。</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -3832,27 +3814,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>9-3</t>
+          <t>9-1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IBM Champion Tech Showcase 体感しよう、技術の進化 #1</t>
+          <t>Meet IBM Research #1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:45-14:55</t>
+          <t>12:45-12:55</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>watsonx.aiとVision Pro連携事例</t>
+          <t>コンピューティングの未来を語ろう</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>このセッションは IBM watsonx.ai と Apple Vision Pro による空間コンピューティングの連携について具体的な手法をライブデモを交えてお伝えします。実践的な実装方法、参考になる注意点、試行錯誤のポイント、AI とデバイスの関係性で感じたことをお伝えします。</t>
+          <t>展示ブース「Meet IBM Research コンピューティングの未来を語ろう」でご案内している最先端テクノロジーの一端をご紹介します。（Meet IBM Research #2 と同じ内容になります。）</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3864,27 +3846,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>9-4</t>
+          <t>9-2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IBM Champion Tech Showcase 体感しよう、技術の進化 #2</t>
+          <t>Meet IBM Research #2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15:45-15:55</t>
+          <t>13:45-13:55</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Call for Code チャレンジ  watsonx.aiとTJBot zero  生成AIアシスタントをつくってみた</t>
+          <t>コンピューティングの未来を語ろう</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>このセッションは、社会問題解決を目指すグローバル・ハッカソン「Call for Code」の2024年テーマ「生成AI」に対応したプロジェクトを紹介します。紙型AIロボット「TJBot Zero」（Raspberry Pi 搭載）を生成AIのフロントエンドとして活用した実践的な応用方法と魅力を解説します。</t>
+          <t>展示ブース「Meet IBM Research コンピューティングの未来を語ろう」でご案内している最先端テクノロジーの一端をご紹介します。（Meet IBM Research #1 と同じ内容になります。）</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3896,27 +3878,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9-5</t>
+          <t>9-3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IBM Champion Tech Showcase 体感しよう、技術の進化 #3</t>
+          <t>IBM Champion Tech Showcase 体感しよう、技術の進化 #1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16:45-16:55</t>
+          <t>14:45-14:55</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Watson Discoveryだから実現できた、業務で使えるAI活用</t>
+          <t>watsonx.aiとVision Pro連携事例</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>業務で生成AIを利用する（=API利用)ためには、ユーザーの質問や指示に対する最適なドキュメントを検索によって抽出し、生成AIに渡す必要があります。ベクトルDBを勧める記事が多くありますが、精度が出にくいこともあります。一方、Watson Discoveryを使う私たちの製品は94%以上の評価を獲得しています。このセッションではデモを交え、Watson DiscoveryがRAGに向いている理由をお伝えします。</t>
+          <t>このセッションは IBM watsonx.ai と Apple Vision Pro による空間コンピューティングの連携について具体的な手法をライブデモを交えてお伝えします。実践的な実装方法、参考になる注意点、試行錯誤のポイント、AI とデバイスの関係性で感じたことをお伝えします。</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3928,27 +3910,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>9-1</t>
+          <t>9-4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Meet IBM Research #1</t>
+          <t>IBM Champion Tech Showcase 体感しよう、技術の進化 #2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12:45-12:55</t>
+          <t>15:45-15:55</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>コンピューティングの未来を語ろう</t>
+          <t>Call for Code チャレンジ  watsonx.aiとTJBot zero  生成AIアシスタントをつくってみた</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>展示ブース「Meet IBM Research コンピューティングの未来を語ろう」でご案内している最先端テクノロジーの一端をご紹介します。（Meet IBM Research #2 と同じ内容になります。）</t>
+          <t>このセッションは、社会問題解決を目指すグローバル・ハッカソン「Call for Code」の2024年テーマ「生成AI」に対応したプロジェクトを紹介します。紙型AIロボット「TJBot Zero」（Raspberry Pi 搭載）を生成AIのフロントエンドとして活用した実践的な応用方法と魅力を解説します。</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3960,27 +3942,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>9-2</t>
+          <t>9-5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Meet IBM Research #2</t>
+          <t>IBM Champion Tech Showcase 体感しよう、技術の進化 #3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>13:45-13:55</t>
+          <t>16:45-16:55</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>コンピューティングの未来を語ろう</t>
+          <t>Watson Discoveryだから実現できた、業務で使えるAI活用</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>展示ブース「Meet IBM Research コンピューティングの未来を語ろう」でご案内している最先端テクノロジーの一端をご紹介します。（Meet IBM Research #1 と同じ内容になります。）</t>
+          <t>業務で生成AIを利用する（=API利用)ためには、ユーザーの質問や指示に対する最適なドキュメントを検索によって抽出し、生成AIに渡す必要があります。ベクトルDBを勧める記事が多くありますが、精度が出にくいこともあります。一方、Watson Discoveryを使う私たちの製品は94%以上の評価を獲得しています。このセッションではデモを交え、Watson DiscoveryがRAGに向いている理由をお伝えします。</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">

</xml_diff>